<commit_message>
Day 1 Excel readme
</commit_message>
<xml_diff>
--- a/excel/2022/day01/Day01.xlsx
+++ b/excel/2022/day01/Day01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\advent-of-code\excel\day01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\advent-of-code\excel\2022\day01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE60236E-1837-4101-84E4-B18A5BF0422C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7E3D44-D12B-4A31-B89E-D4B9A2537888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F7898A9C-4E7C-43D8-8F1E-886D8EF850EC}"/>
+    <workbookView xWindow="-28920" yWindow="2835" windowWidth="29040" windowHeight="15840" xr2:uid="{F7898A9C-4E7C-43D8-8F1E-886D8EF850EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
   <dimension ref="A1:H2277"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -488,11 +488,11 @@
         <v>8782</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B41" si="0">IF(A4,A4+B3,)</f>
+        <f t="shared" ref="B4:B40" si="0">IF(A4,A4+B3,)</f>
         <v>24713</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C41" si="1">IF(B5,,B4)</f>
+        <f t="shared" ref="C4:C39" si="1">IF(B5,,B4)</f>
         <v>0</v>
       </c>
       <c r="E4">

</xml_diff>